<commit_message>
small fix with wards/bydeler
</commit_message>
<xml_diff>
--- a/inst/extdata/norway_locations_ward.xlsx
+++ b/inst/extdata/norway_locations_ward.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riwh\OneDrive - Folkehelseinstituttet\packages\fhidata\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{E0AA4139-EC72-7240-B4DA-8072FE8D2BA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D31FB950-7E11-4BD4-8D2E-CF139CEFCE6D}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{E0AA4139-EC72-7240-B4DA-8072FE8D2BA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{889E747B-1AC2-44FA-8DF2-C45249297EDE}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="norwayLocations" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Østensjø</t>
   </si>
   <si>
-    <t>county03</t>
-  </si>
-  <si>
     <t>Oslo</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>ward030113</t>
+  </si>
+  <si>
+    <t>municip0301</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G2" sqref="G2:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="1023" width="10.42578125" customWidth="1"/>
   </cols>
@@ -535,10 +535,10 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -549,16 +549,16 @@
         <v>2005</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -566,16 +566,16 @@
         <v>2005</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -583,16 +583,16 @@
         <v>2005</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -600,16 +600,16 @@
         <v>2005</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -617,16 +617,16 @@
         <v>2005</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -634,16 +634,16 @@
         <v>2005</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -651,16 +651,16 @@
         <v>2005</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -668,16 +668,16 @@
         <v>2005</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,16 +685,16 @@
         <v>2005</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -702,16 +702,16 @@
         <v>2005</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,16 +719,16 @@
         <v>2005</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -736,16 +736,16 @@
         <v>2005</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -753,16 +753,16 @@
         <v>2005</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -770,16 +770,16 @@
         <v>2005</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,16 +787,16 @@
         <v>2005</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>